<commit_message>
Add graph relationship when connect
</commit_message>
<xml_diff>
--- a/資料庫範例.xlsx
+++ b/資料庫範例.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\project\vs2017_project\PyQT_test\ITRI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H200\PyQt5_Gui_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{4A24FA98-31D1-4A75-A7F4-5252A55BEC0C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="管理系統(範本)" sheetId="2" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>委辦單位</t>
   </si>
@@ -295,11 +294,15 @@
     <t>台灣</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>件編號普浪</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -530,10 +533,10 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="一般_工作表2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="一般_工作表4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="一般_加值紀錄" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="一般 2" xfId="1"/>
+    <cellStyle name="一般_工作表2" xfId="2"/>
+    <cellStyle name="一般_工作表4" xfId="3"/>
+    <cellStyle name="一般_加值紀錄" xfId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -810,10 +813,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="C2" sqref="C2"/>
     </sheetView>
@@ -1472,10 +1475,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1484,7 +1487,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>2</v>
+        <v>80</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>31</v>
@@ -1609,7 +1612,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFC23"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -18582,7 +18585,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>

</xml_diff>

<commit_message>
Finish output loops without implementing generateOut
</commit_message>
<xml_diff>
--- a/資料庫範例.xlsx
+++ b/資料庫範例.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\H200\PyQt5_Gui_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\project\vs2017_project\PyQT_test\ITRI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{543E7993-60C8-4D79-85C5-44DC13493078}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="管理系統(範本)" sheetId="2" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
   <si>
     <t>委辦單位</t>
   </si>
@@ -298,11 +299,15 @@
     <t>件編號普浪</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>YO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -533,10 +538,10 @@
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2" xfId="1"/>
-    <cellStyle name="一般_工作表2" xfId="2"/>
-    <cellStyle name="一般_工作表4" xfId="3"/>
-    <cellStyle name="一般_加值紀錄" xfId="4"/>
+    <cellStyle name="一般 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="一般_工作表2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="一般_工作表4" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="一般_加值紀錄" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -813,12 +818,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AJ15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2"/>
+      <selection pane="topRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -949,8 +954,8 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
-        <v>12</v>
+      <c r="B2" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="C2" s="4">
         <v>212021321</v>
@@ -1475,10 +1480,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1612,7 +1617,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:XFC23"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
@@ -18585,7 +18590,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>

</xml_diff>